<commit_message>
update U souhaitable PBQ
</commit_message>
<xml_diff>
--- a/EFLM_2025.xlsx
+++ b/EFLM_2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cornet-e\GITHUB\CV-IM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7391430-57BF-4390-8013-62E94C3A751F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8660F029-487E-4466-9919-DBE97B4702CD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="27825" windowHeight="12210" xr2:uid="{86864417-4E27-4685-A4E2-9D59210BA540}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="58">
   <si>
     <t>Cva_min</t>
   </si>
@@ -190,6 +190,15 @@
   </si>
   <si>
     <t>Mean corpuscular haemoglobin (MCH)</t>
+  </si>
+  <si>
+    <t>U_souhaitable_PBQ</t>
+  </si>
+  <si>
+    <t>MCHC(g/dL)</t>
+  </si>
+  <si>
+    <t>MCH(pg)</t>
   </si>
 </sst>
 </file>
@@ -197,7 +206,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -308,18 +317,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -341,13 +350,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>18</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
+      <xdr:col>27</xdr:col>
       <xdr:colOff>734377</xdr:colOff>
       <xdr:row>53</xdr:row>
       <xdr:rowOff>163121</xdr:rowOff>
@@ -683,10 +692,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C50B7B0-1553-4E40-94BB-F3DD0E6A8175}">
-  <dimension ref="A1:T22"/>
+  <dimension ref="A1:U22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -700,9 +709,10 @@
     <col min="9" max="9" width="11.42578125" style="6"/>
     <col min="13" max="13" width="11.42578125" style="6"/>
     <col min="17" max="18" width="11.42578125" style="6"/>
+    <col min="19" max="19" width="11.42578125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>50</v>
       </c>
@@ -754,9 +764,11 @@
       <c r="Q1" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="R1" s="10"/>
+      <c r="R1" s="10" t="s">
+        <v>55</v>
+      </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -820,8 +832,11 @@
       <c r="Q2" s="6">
         <v>2</v>
       </c>
+      <c r="R2" s="6">
+        <v>14.8</v>
+      </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -885,8 +900,11 @@
       <c r="Q3" s="6">
         <v>2</v>
       </c>
+      <c r="R3" s="6">
+        <v>4.5999999999999996</v>
+      </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>41</v>
       </c>
@@ -950,8 +968,11 @@
       <c r="Q4" s="6">
         <v>2</v>
       </c>
+      <c r="R4" s="6">
+        <v>2.9</v>
+      </c>
     </row>
-    <row r="5" spans="1:20" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -1015,14 +1036,17 @@
       <c r="Q5" s="6">
         <v>2</v>
       </c>
-      <c r="S5" t="s">
+      <c r="R5" s="6">
+        <v>4.3</v>
+      </c>
+      <c r="T5" t="s">
         <v>25</v>
       </c>
-      <c r="T5" s="3" t="s">
+      <c r="U5" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -1086,18 +1110,23 @@
       <c r="Q6" s="6">
         <v>2</v>
       </c>
-      <c r="S6" t="s">
+      <c r="R6" s="6">
+        <v>4.2</v>
+      </c>
+      <c r="T6" t="s">
         <v>26</v>
       </c>
-      <c r="T6" s="3" t="s">
+      <c r="U6" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="C7" s="6">
         <v>0.7</v>
       </c>
@@ -1155,13 +1184,18 @@
       <c r="Q7" s="6">
         <v>2</v>
       </c>
-      <c r="T7" s="3"/>
+      <c r="R7" s="6">
+        <v>2.5</v>
+      </c>
+      <c r="U7" s="3"/>
     </row>
-    <row r="8" spans="1:20" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>53</v>
       </c>
-      <c r="B8" s="1"/>
+      <c r="B8" s="1" t="s">
+        <v>56</v>
+      </c>
       <c r="C8" s="6">
         <v>1</v>
       </c>
@@ -1219,9 +1253,12 @@
       <c r="Q8" s="6">
         <v>2</v>
       </c>
-      <c r="T8" s="3"/>
+      <c r="R8" s="6">
+        <v>1.3</v>
+      </c>
+      <c r="U8" s="3"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -1243,7 +1280,7 @@
         <v>7.4929654510080326</v>
       </c>
       <c r="G9" s="12">
-        <f>Q9*0.75*C9</f>
+        <f t="shared" ref="G9:G22" si="30">Q9*0.75*C9</f>
         <v>10.95</v>
       </c>
       <c r="H9" s="5">
@@ -1259,7 +1296,7 @@
         <v>4.9953103006720214</v>
       </c>
       <c r="K9" s="13">
-        <f>Q9*0.5*C9</f>
+        <f t="shared" ref="K9:K22" si="31">Q9*0.5*C9</f>
         <v>7.3</v>
       </c>
       <c r="L9" s="2">
@@ -1275,7 +1312,7 @@
         <v>2.4976551503360107</v>
       </c>
       <c r="O9" s="13">
-        <f>Q9*0.25*C9</f>
+        <f t="shared" ref="O9:O22" si="32">Q9*0.25*C9</f>
         <v>3.65</v>
       </c>
       <c r="P9" s="2">
@@ -1285,8 +1322,11 @@
       <c r="Q9" s="6">
         <v>2</v>
       </c>
+      <c r="R9" s="6">
+        <v>11.4</v>
+      </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -1308,7 +1348,7 @@
         <v>7.4929654510080326</v>
       </c>
       <c r="G10" s="12">
-        <f>Q10*0.75*C10</f>
+        <f t="shared" si="30"/>
         <v>10.95</v>
       </c>
       <c r="H10" s="5">
@@ -1324,7 +1364,7 @@
         <v>4.9953103006720214</v>
       </c>
       <c r="K10" s="13">
-        <f>Q10*0.5*C10</f>
+        <f t="shared" si="31"/>
         <v>7.3</v>
       </c>
       <c r="L10" s="2">
@@ -1340,7 +1380,7 @@
         <v>2.4976551503360107</v>
       </c>
       <c r="O10" s="13">
-        <f>Q10*0.25*C10</f>
+        <f t="shared" si="32"/>
         <v>3.65</v>
       </c>
       <c r="P10" s="2">
@@ -1350,8 +1390,11 @@
       <c r="Q10" s="6">
         <v>2</v>
       </c>
+      <c r="R10" s="6">
+        <v>11.4</v>
+      </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -1365,58 +1408,61 @@
         <v>7.1</v>
       </c>
       <c r="E11" s="4">
-        <f t="shared" ref="E11:E22" si="30">0.75*C11</f>
+        <f t="shared" ref="E11:E22" si="33">0.75*C11</f>
         <v>1.7249999999999999</v>
       </c>
       <c r="F11" s="5">
-        <f t="shared" ref="F11:F22" si="31">0.375*SQRT((C11^2+D11^2))</f>
+        <f t="shared" ref="F11:F22" si="34">0.375*SQRT((C11^2+D11^2))</f>
         <v>2.7987162235567933</v>
       </c>
       <c r="G11" s="12">
-        <f>Q11*0.75*C11</f>
+        <f t="shared" si="30"/>
         <v>3.4499999999999997</v>
       </c>
       <c r="H11" s="5">
-        <f t="shared" ref="H11:H22" si="32">1.65*E11+F11</f>
+        <f t="shared" ref="H11:H22" si="35">1.65*E11+F11</f>
         <v>5.6449662235567928</v>
       </c>
       <c r="I11" s="4">
-        <f t="shared" ref="I11:I22" si="33">0.5*C11</f>
+        <f t="shared" ref="I11:I22" si="36">0.5*C11</f>
         <v>1.1499999999999999</v>
       </c>
       <c r="J11" s="2">
-        <f t="shared" ref="J11:J22" si="34">0.25*SQRT((C11^2+D11^2))</f>
+        <f t="shared" ref="J11:J22" si="37">0.25*SQRT((C11^2+D11^2))</f>
         <v>1.865810815704529</v>
       </c>
       <c r="K11" s="13">
-        <f>Q11*0.5*C11</f>
+        <f t="shared" si="31"/>
         <v>2.2999999999999998</v>
       </c>
       <c r="L11" s="2">
-        <f t="shared" ref="L11:L22" si="35">1.65*I11+J11</f>
+        <f t="shared" ref="L11:L22" si="38">1.65*I11+J11</f>
         <v>3.7633108157045285</v>
       </c>
       <c r="M11" s="4">
-        <f t="shared" ref="M11:M22" si="36">0.25*C11</f>
+        <f t="shared" ref="M11:M22" si="39">0.25*C11</f>
         <v>0.57499999999999996</v>
       </c>
       <c r="N11" s="2">
-        <f t="shared" ref="N11:N22" si="37">0.125*SQRT((C11^2+D11^2))</f>
+        <f t="shared" ref="N11:N22" si="40">0.125*SQRT((C11^2+D11^2))</f>
         <v>0.9329054078522645</v>
       </c>
       <c r="O11" s="13">
-        <f>Q11*0.25*C11</f>
+        <f t="shared" si="32"/>
         <v>1.1499999999999999</v>
       </c>
       <c r="P11" s="2">
-        <f t="shared" ref="P11:P22" si="38">1.65*M11+N11</f>
+        <f t="shared" ref="P11:P22" si="41">1.65*M11+N11</f>
         <v>1.8816554078522643</v>
       </c>
       <c r="Q11" s="6">
         <v>2</v>
       </c>
+      <c r="R11" s="6">
+        <v>4.4000000000000004</v>
+      </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -1428,58 +1474,58 @@
         <v>13.5</v>
       </c>
       <c r="E12" s="4">
+        <f t="shared" si="33"/>
+        <v>4.8000000000000007</v>
+      </c>
+      <c r="F12" s="5">
+        <f t="shared" si="34"/>
+        <v>5.6025803207093778</v>
+      </c>
+      <c r="G12" s="12">
         <f t="shared" si="30"/>
-        <v>4.8000000000000007</v>
-      </c>
-      <c r="F12" s="5">
+        <v>9.6000000000000014</v>
+      </c>
+      <c r="H12" s="5">
+        <f t="shared" si="35"/>
+        <v>13.522580320709379</v>
+      </c>
+      <c r="I12" s="4">
+        <f t="shared" si="36"/>
+        <v>3.2</v>
+      </c>
+      <c r="J12" s="2">
+        <f t="shared" si="37"/>
+        <v>3.7350535471395854</v>
+      </c>
+      <c r="K12" s="13">
         <f t="shared" si="31"/>
-        <v>5.6025803207093778</v>
-      </c>
-      <c r="G12" s="12">
-        <f>Q12*0.75*C12</f>
-        <v>9.6000000000000014</v>
-      </c>
-      <c r="H12" s="5">
+        <v>6.4</v>
+      </c>
+      <c r="L12" s="2">
+        <f t="shared" si="38"/>
+        <v>9.0150535471395852</v>
+      </c>
+      <c r="M12" s="4">
+        <f t="shared" si="39"/>
+        <v>1.6</v>
+      </c>
+      <c r="N12" s="2">
+        <f t="shared" si="40"/>
+        <v>1.8675267735697927</v>
+      </c>
+      <c r="O12" s="13">
         <f t="shared" si="32"/>
-        <v>13.522580320709379</v>
-      </c>
-      <c r="I12" s="4">
-        <f t="shared" si="33"/>
         <v>3.2</v>
       </c>
-      <c r="J12" s="2">
-        <f t="shared" si="34"/>
-        <v>3.7350535471395854</v>
-      </c>
-      <c r="K12" s="13">
-        <f>Q12*0.5*C12</f>
-        <v>6.4</v>
-      </c>
-      <c r="L12" s="2">
-        <f t="shared" si="35"/>
-        <v>9.0150535471395852</v>
-      </c>
-      <c r="M12" s="4">
-        <f t="shared" si="36"/>
-        <v>1.6</v>
-      </c>
-      <c r="N12" s="2">
-        <f t="shared" si="37"/>
-        <v>1.8675267735697927</v>
-      </c>
-      <c r="O12" s="13">
-        <f>Q12*0.25*C12</f>
-        <v>3.2</v>
-      </c>
       <c r="P12" s="2">
-        <f t="shared" si="38"/>
+        <f t="shared" si="41"/>
         <v>4.5075267735697926</v>
       </c>
       <c r="Q12" s="6">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -1491,58 +1537,58 @@
         <v>12.3</v>
       </c>
       <c r="E13" s="4">
+        <f t="shared" si="33"/>
+        <v>2.8499999999999996</v>
+      </c>
+      <c r="F13" s="5">
+        <f t="shared" si="34"/>
+        <v>4.8276061614427501</v>
+      </c>
+      <c r="G13" s="12">
         <f t="shared" si="30"/>
-        <v>2.8499999999999996</v>
-      </c>
-      <c r="F13" s="5">
+        <v>5.6999999999999993</v>
+      </c>
+      <c r="H13" s="5">
+        <f t="shared" si="35"/>
+        <v>9.5301061614427489</v>
+      </c>
+      <c r="I13" s="4">
+        <f t="shared" si="36"/>
+        <v>1.9</v>
+      </c>
+      <c r="J13" s="2">
+        <f t="shared" si="37"/>
+        <v>3.2184041076284999</v>
+      </c>
+      <c r="K13" s="13">
         <f t="shared" si="31"/>
-        <v>4.8276061614427501</v>
-      </c>
-      <c r="G13" s="12">
-        <f>Q13*0.75*C13</f>
-        <v>5.6999999999999993</v>
-      </c>
-      <c r="H13" s="5">
+        <v>3.8</v>
+      </c>
+      <c r="L13" s="2">
+        <f t="shared" si="38"/>
+        <v>6.3534041076284993</v>
+      </c>
+      <c r="M13" s="4">
+        <f t="shared" si="39"/>
+        <v>0.95</v>
+      </c>
+      <c r="N13" s="2">
+        <f t="shared" si="40"/>
+        <v>1.60920205381425</v>
+      </c>
+      <c r="O13" s="13">
         <f t="shared" si="32"/>
-        <v>9.5301061614427489</v>
-      </c>
-      <c r="I13" s="4">
-        <f t="shared" si="33"/>
         <v>1.9</v>
       </c>
-      <c r="J13" s="2">
-        <f t="shared" si="34"/>
-        <v>3.2184041076284999</v>
-      </c>
-      <c r="K13" s="13">
-        <f>Q13*0.5*C13</f>
-        <v>3.8</v>
-      </c>
-      <c r="L13" s="2">
-        <f t="shared" si="35"/>
-        <v>6.3534041076284993</v>
-      </c>
-      <c r="M13" s="4">
-        <f t="shared" si="36"/>
-        <v>0.95</v>
-      </c>
-      <c r="N13" s="2">
-        <f t="shared" si="37"/>
-        <v>1.60920205381425</v>
-      </c>
-      <c r="O13" s="13">
-        <f>Q13*0.25*C13</f>
-        <v>1.9</v>
-      </c>
       <c r="P13" s="2">
-        <f t="shared" si="38"/>
+        <f t="shared" si="41"/>
         <v>3.1767020538142496</v>
       </c>
       <c r="Q13" s="6">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -1554,58 +1600,58 @@
         <v>20.9</v>
       </c>
       <c r="E14" s="4">
+        <f t="shared" si="33"/>
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="F14" s="5">
+        <f t="shared" si="34"/>
+        <v>8.2418994321697472</v>
+      </c>
+      <c r="G14" s="12">
         <f t="shared" si="30"/>
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="F14" s="5">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="H14" s="5">
+        <f t="shared" si="35"/>
+        <v>16.656899432169745</v>
+      </c>
+      <c r="I14" s="4">
+        <f t="shared" si="36"/>
+        <v>3.4</v>
+      </c>
+      <c r="J14" s="2">
+        <f t="shared" si="37"/>
+        <v>5.4945996214464978</v>
+      </c>
+      <c r="K14" s="13">
         <f t="shared" si="31"/>
-        <v>8.2418994321697472</v>
-      </c>
-      <c r="G14" s="12">
-        <f>Q14*0.75*C14</f>
-        <v>10.199999999999999</v>
-      </c>
-      <c r="H14" s="5">
+        <v>6.8</v>
+      </c>
+      <c r="L14" s="2">
+        <f t="shared" si="38"/>
+        <v>11.104599621446496</v>
+      </c>
+      <c r="M14" s="4">
+        <f t="shared" si="39"/>
+        <v>1.7</v>
+      </c>
+      <c r="N14" s="2">
+        <f t="shared" si="40"/>
+        <v>2.7472998107232489</v>
+      </c>
+      <c r="O14" s="13">
         <f t="shared" si="32"/>
-        <v>16.656899432169745</v>
-      </c>
-      <c r="I14" s="4">
-        <f t="shared" si="33"/>
         <v>3.4</v>
       </c>
-      <c r="J14" s="2">
-        <f t="shared" si="34"/>
-        <v>5.4945996214464978</v>
-      </c>
-      <c r="K14" s="13">
-        <f>Q14*0.5*C14</f>
-        <v>6.8</v>
-      </c>
-      <c r="L14" s="2">
-        <f t="shared" si="35"/>
-        <v>11.104599621446496</v>
-      </c>
-      <c r="M14" s="4">
-        <f t="shared" si="36"/>
-        <v>1.7</v>
-      </c>
-      <c r="N14" s="2">
-        <f t="shared" si="37"/>
-        <v>2.7472998107232489</v>
-      </c>
-      <c r="O14" s="13">
-        <f>Q14*0.25*C14</f>
-        <v>3.4</v>
-      </c>
       <c r="P14" s="2">
-        <f t="shared" si="38"/>
+        <f t="shared" si="41"/>
         <v>5.5522998107232482</v>
       </c>
       <c r="Q14" s="6">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>38</v>
       </c>
@@ -1619,58 +1665,58 @@
         <v>27.1</v>
       </c>
       <c r="E15" s="4">
+        <f t="shared" si="33"/>
+        <v>7.2749999999999995</v>
+      </c>
+      <c r="F15" s="5">
+        <f t="shared" si="34"/>
+        <v>10.79387847346819</v>
+      </c>
+      <c r="G15" s="12">
         <f t="shared" si="30"/>
-        <v>7.2749999999999995</v>
-      </c>
-      <c r="F15" s="5">
+        <v>14.549999999999999</v>
+      </c>
+      <c r="H15" s="5">
+        <f t="shared" si="35"/>
+        <v>22.797628473468187</v>
+      </c>
+      <c r="I15" s="4">
+        <f t="shared" si="36"/>
+        <v>4.8499999999999996</v>
+      </c>
+      <c r="J15" s="2">
+        <f t="shared" si="37"/>
+        <v>7.1959189823121275</v>
+      </c>
+      <c r="K15" s="13">
         <f t="shared" si="31"/>
-        <v>10.79387847346819</v>
-      </c>
-      <c r="G15" s="12">
-        <f>Q15*0.75*C15</f>
-        <v>14.549999999999999</v>
-      </c>
-      <c r="H15" s="5">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="L15" s="2">
+        <f t="shared" si="38"/>
+        <v>15.198418982312127</v>
+      </c>
+      <c r="M15" s="4">
+        <f t="shared" si="39"/>
+        <v>2.4249999999999998</v>
+      </c>
+      <c r="N15" s="2">
+        <f t="shared" si="40"/>
+        <v>3.5979594911560637</v>
+      </c>
+      <c r="O15" s="13">
         <f t="shared" si="32"/>
-        <v>22.797628473468187</v>
-      </c>
-      <c r="I15" s="4">
-        <f t="shared" si="33"/>
         <v>4.8499999999999996</v>
       </c>
-      <c r="J15" s="2">
-        <f t="shared" si="34"/>
-        <v>7.1959189823121275</v>
-      </c>
-      <c r="K15" s="13">
-        <f>Q15*0.5*C15</f>
-        <v>9.6999999999999993</v>
-      </c>
-      <c r="L15" s="2">
-        <f t="shared" si="35"/>
-        <v>15.198418982312127</v>
-      </c>
-      <c r="M15" s="4">
-        <f t="shared" si="36"/>
-        <v>2.4249999999999998</v>
-      </c>
-      <c r="N15" s="2">
-        <f t="shared" si="37"/>
-        <v>3.5979594911560637</v>
-      </c>
-      <c r="O15" s="13">
-        <f>Q15*0.25*C15</f>
-        <v>4.8499999999999996</v>
-      </c>
       <c r="P15" s="2">
-        <f t="shared" si="38"/>
+        <f t="shared" si="41"/>
         <v>7.5992094911560635</v>
       </c>
       <c r="Q15" s="6">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>39</v>
       </c>
@@ -1684,58 +1730,58 @@
         <v>3.4</v>
       </c>
       <c r="E16" s="4">
+        <f t="shared" si="33"/>
+        <v>1.2749999999999999</v>
+      </c>
+      <c r="F16" s="5">
+        <f t="shared" si="34"/>
+        <v>1.4254933356561159</v>
+      </c>
+      <c r="G16" s="12">
         <f t="shared" si="30"/>
-        <v>1.2749999999999999</v>
-      </c>
-      <c r="F16" s="5">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="H16" s="5">
+        <f t="shared" si="35"/>
+        <v>3.5292433356561155</v>
+      </c>
+      <c r="I16" s="4">
+        <f t="shared" si="36"/>
+        <v>0.85</v>
+      </c>
+      <c r="J16" s="2">
+        <f t="shared" si="37"/>
+        <v>0.95032889043741064</v>
+      </c>
+      <c r="K16" s="13">
         <f t="shared" si="31"/>
-        <v>1.4254933356561159</v>
-      </c>
-      <c r="G16" s="12">
-        <f>Q16*0.75*C16</f>
-        <v>2.5499999999999998</v>
-      </c>
-      <c r="H16" s="5">
+        <v>1.7</v>
+      </c>
+      <c r="L16" s="2">
+        <f t="shared" si="38"/>
+        <v>2.3528288904374106</v>
+      </c>
+      <c r="M16" s="4">
+        <f t="shared" si="39"/>
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="N16" s="2">
+        <f t="shared" si="40"/>
+        <v>0.47516444521870532</v>
+      </c>
+      <c r="O16" s="13">
         <f t="shared" si="32"/>
-        <v>3.5292433356561155</v>
-      </c>
-      <c r="I16" s="4">
-        <f t="shared" si="33"/>
         <v>0.85</v>
       </c>
-      <c r="J16" s="2">
-        <f t="shared" si="34"/>
-        <v>0.95032889043741064</v>
-      </c>
-      <c r="K16" s="13">
-        <f>Q16*0.5*C16</f>
-        <v>1.7</v>
-      </c>
-      <c r="L16" s="2">
-        <f t="shared" si="35"/>
-        <v>2.3528288904374106</v>
-      </c>
-      <c r="M16" s="4">
-        <f t="shared" si="36"/>
-        <v>0.42499999999999999</v>
-      </c>
-      <c r="N16" s="2">
-        <f t="shared" si="37"/>
-        <v>0.47516444521870532</v>
-      </c>
-      <c r="O16" s="13">
-        <f>Q16*0.25*C16</f>
-        <v>0.85</v>
-      </c>
       <c r="P16" s="2">
-        <f t="shared" si="38"/>
+        <f t="shared" si="41"/>
         <v>1.1764144452187053</v>
       </c>
       <c r="Q16" s="6">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -1749,58 +1795,61 @@
         <v>3.9</v>
       </c>
       <c r="E17" s="4">
+        <f t="shared" si="33"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="F17" s="5">
+        <f t="shared" si="34"/>
+        <v>1.4929521928045788</v>
+      </c>
+      <c r="G17" s="12">
         <f t="shared" si="30"/>
-        <v>0.60000000000000009</v>
-      </c>
-      <c r="F17" s="5">
+        <v>1.2000000000000002</v>
+      </c>
+      <c r="H17" s="5">
+        <f t="shared" si="35"/>
+        <v>2.482952192804579</v>
+      </c>
+      <c r="I17" s="4">
+        <f t="shared" si="36"/>
+        <v>0.4</v>
+      </c>
+      <c r="J17" s="2">
+        <f t="shared" si="37"/>
+        <v>0.99530146186971913</v>
+      </c>
+      <c r="K17" s="13">
         <f t="shared" si="31"/>
-        <v>1.4929521928045788</v>
-      </c>
-      <c r="G17" s="12">
-        <f>Q17*0.75*C17</f>
-        <v>1.2000000000000002</v>
-      </c>
-      <c r="H17" s="5">
+        <v>0.8</v>
+      </c>
+      <c r="L17" s="2">
+        <f t="shared" si="38"/>
+        <v>1.655301461869719</v>
+      </c>
+      <c r="M17" s="4">
+        <f t="shared" si="39"/>
+        <v>0.2</v>
+      </c>
+      <c r="N17" s="2">
+        <f t="shared" si="40"/>
+        <v>0.49765073093485956</v>
+      </c>
+      <c r="O17" s="13">
         <f t="shared" si="32"/>
-        <v>2.482952192804579</v>
-      </c>
-      <c r="I17" s="4">
-        <f t="shared" si="33"/>
         <v>0.4</v>
       </c>
-      <c r="J17" s="2">
-        <f t="shared" si="34"/>
-        <v>0.99530146186971913</v>
-      </c>
-      <c r="K17" s="13">
-        <f>Q17*0.5*C17</f>
-        <v>0.8</v>
-      </c>
-      <c r="L17" s="2">
-        <f t="shared" si="35"/>
-        <v>1.655301461869719</v>
-      </c>
-      <c r="M17" s="4">
-        <f t="shared" si="36"/>
-        <v>0.2</v>
-      </c>
-      <c r="N17" s="2">
-        <f t="shared" si="37"/>
-        <v>0.49765073093485956</v>
-      </c>
-      <c r="O17" s="13">
-        <f>Q17*0.25*C17</f>
-        <v>0.4</v>
-      </c>
       <c r="P17" s="2">
-        <f t="shared" si="38"/>
+        <f t="shared" si="41"/>
         <v>0.82765073093485952</v>
       </c>
       <c r="Q17" s="6">
         <v>2</v>
       </c>
+      <c r="R17" s="6">
+        <v>2.1</v>
+      </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>42</v>
       </c>
@@ -1814,58 +1863,58 @@
         <v>22.8</v>
       </c>
       <c r="E18" s="4">
+        <f t="shared" si="33"/>
+        <v>7.875</v>
+      </c>
+      <c r="F18" s="5">
+        <f t="shared" si="34"/>
+        <v>9.4130975905915264</v>
+      </c>
+      <c r="G18" s="12">
         <f t="shared" si="30"/>
-        <v>7.875</v>
-      </c>
-      <c r="F18" s="5">
+        <v>15.75</v>
+      </c>
+      <c r="H18" s="5">
+        <f t="shared" si="35"/>
+        <v>22.406847590591525</v>
+      </c>
+      <c r="I18" s="4">
+        <f t="shared" si="36"/>
+        <v>5.25</v>
+      </c>
+      <c r="J18" s="2">
+        <f t="shared" si="37"/>
+        <v>6.2753983937276843</v>
+      </c>
+      <c r="K18" s="13">
         <f t="shared" si="31"/>
-        <v>9.4130975905915264</v>
-      </c>
-      <c r="G18" s="12">
-        <f>Q18*0.75*C18</f>
-        <v>15.75</v>
-      </c>
-      <c r="H18" s="5">
+        <v>10.5</v>
+      </c>
+      <c r="L18" s="2">
+        <f t="shared" si="38"/>
+        <v>14.937898393727684</v>
+      </c>
+      <c r="M18" s="4">
+        <f t="shared" si="39"/>
+        <v>2.625</v>
+      </c>
+      <c r="N18" s="2">
+        <f t="shared" si="40"/>
+        <v>3.1376991968638421</v>
+      </c>
+      <c r="O18" s="13">
         <f t="shared" si="32"/>
-        <v>22.406847590591525</v>
-      </c>
-      <c r="I18" s="4">
-        <f t="shared" si="33"/>
         <v>5.25</v>
       </c>
-      <c r="J18" s="2">
-        <f t="shared" si="34"/>
-        <v>6.2753983937276843</v>
-      </c>
-      <c r="K18" s="13">
-        <f>Q18*0.5*C18</f>
-        <v>10.5</v>
-      </c>
-      <c r="L18" s="2">
-        <f t="shared" si="35"/>
-        <v>14.937898393727684</v>
-      </c>
-      <c r="M18" s="4">
-        <f t="shared" si="36"/>
-        <v>2.625</v>
-      </c>
-      <c r="N18" s="2">
-        <f t="shared" si="37"/>
-        <v>3.1376991968638421</v>
-      </c>
-      <c r="O18" s="13">
-        <f>Q18*0.25*C18</f>
-        <v>5.25</v>
-      </c>
       <c r="P18" s="2">
-        <f t="shared" si="38"/>
+        <f t="shared" si="41"/>
         <v>7.468949196863842</v>
       </c>
       <c r="Q18" s="6">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -1879,58 +1928,58 @@
         <v>23</v>
       </c>
       <c r="E19" s="4">
+        <f t="shared" si="33"/>
+        <v>10.5</v>
+      </c>
+      <c r="F19" s="5">
+        <f t="shared" si="34"/>
+        <v>10.097184013377195</v>
+      </c>
+      <c r="G19" s="12">
         <f t="shared" si="30"/>
-        <v>10.5</v>
-      </c>
-      <c r="F19" s="5">
+        <v>21</v>
+      </c>
+      <c r="H19" s="5">
+        <f t="shared" si="35"/>
+        <v>27.422184013377194</v>
+      </c>
+      <c r="I19" s="4">
+        <f t="shared" si="36"/>
+        <v>7</v>
+      </c>
+      <c r="J19" s="2">
+        <f t="shared" si="37"/>
+        <v>6.7314560089181299</v>
+      </c>
+      <c r="K19" s="13">
         <f t="shared" si="31"/>
-        <v>10.097184013377195</v>
-      </c>
-      <c r="G19" s="12">
-        <f>Q19*0.75*C19</f>
-        <v>21</v>
-      </c>
-      <c r="H19" s="5">
+        <v>14</v>
+      </c>
+      <c r="L19" s="2">
+        <f t="shared" si="38"/>
+        <v>18.281456008918127</v>
+      </c>
+      <c r="M19" s="4">
+        <f t="shared" si="39"/>
+        <v>3.5</v>
+      </c>
+      <c r="N19" s="2">
+        <f t="shared" si="40"/>
+        <v>3.3657280044590649</v>
+      </c>
+      <c r="O19" s="13">
         <f t="shared" si="32"/>
-        <v>27.422184013377194</v>
-      </c>
-      <c r="I19" s="4">
-        <f t="shared" si="33"/>
         <v>7</v>
       </c>
-      <c r="J19" s="2">
-        <f t="shared" si="34"/>
-        <v>6.7314560089181299</v>
-      </c>
-      <c r="K19" s="13">
-        <f>Q19*0.5*C19</f>
-        <v>14</v>
-      </c>
-      <c r="L19" s="2">
-        <f t="shared" si="35"/>
-        <v>18.281456008918127</v>
-      </c>
-      <c r="M19" s="4">
-        <f t="shared" si="36"/>
-        <v>3.5</v>
-      </c>
-      <c r="N19" s="2">
-        <f t="shared" si="37"/>
-        <v>3.3657280044590649</v>
-      </c>
-      <c r="O19" s="13">
-        <f>Q19*0.25*C19</f>
-        <v>7</v>
-      </c>
       <c r="P19" s="2">
-        <f t="shared" si="38"/>
+        <f t="shared" si="41"/>
         <v>9.1407280044590635</v>
       </c>
       <c r="Q19" s="6">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>44</v>
       </c>
@@ -1944,58 +1993,58 @@
         <v>28.6</v>
       </c>
       <c r="E20" s="4">
+        <f t="shared" si="33"/>
+        <v>9.4499999999999993</v>
+      </c>
+      <c r="F20" s="5">
+        <f t="shared" si="34"/>
+        <v>11.719694961900672</v>
+      </c>
+      <c r="G20" s="12">
         <f t="shared" si="30"/>
-        <v>9.4499999999999993</v>
-      </c>
-      <c r="F20" s="5">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="H20" s="5">
+        <f t="shared" si="35"/>
+        <v>27.312194961900669</v>
+      </c>
+      <c r="I20" s="4">
+        <f t="shared" si="36"/>
+        <v>6.3</v>
+      </c>
+      <c r="J20" s="2">
+        <f t="shared" si="37"/>
+        <v>7.8131299746004483</v>
+      </c>
+      <c r="K20" s="13">
         <f t="shared" si="31"/>
-        <v>11.719694961900672</v>
-      </c>
-      <c r="G20" s="12">
-        <f>Q20*0.75*C20</f>
-        <v>18.899999999999999</v>
-      </c>
-      <c r="H20" s="5">
+        <v>12.6</v>
+      </c>
+      <c r="L20" s="2">
+        <f t="shared" si="38"/>
+        <v>18.208129974600446</v>
+      </c>
+      <c r="M20" s="4">
+        <f t="shared" si="39"/>
+        <v>3.15</v>
+      </c>
+      <c r="N20" s="2">
+        <f t="shared" si="40"/>
+        <v>3.9065649873002242</v>
+      </c>
+      <c r="O20" s="13">
         <f t="shared" si="32"/>
-        <v>27.312194961900669</v>
-      </c>
-      <c r="I20" s="4">
-        <f t="shared" si="33"/>
         <v>6.3</v>
       </c>
-      <c r="J20" s="2">
-        <f t="shared" si="34"/>
-        <v>7.8131299746004483</v>
-      </c>
-      <c r="K20" s="13">
-        <f>Q20*0.5*C20</f>
-        <v>12.6</v>
-      </c>
-      <c r="L20" s="2">
-        <f t="shared" si="35"/>
-        <v>18.208129974600446</v>
-      </c>
-      <c r="M20" s="4">
-        <f t="shared" si="36"/>
-        <v>3.15</v>
-      </c>
-      <c r="N20" s="2">
-        <f t="shared" si="37"/>
-        <v>3.9065649873002242</v>
-      </c>
-      <c r="O20" s="13">
-        <f>Q20*0.25*C20</f>
-        <v>6.3</v>
-      </c>
       <c r="P20" s="2">
-        <f t="shared" si="38"/>
+        <f t="shared" si="41"/>
         <v>9.1040649873002231</v>
       </c>
       <c r="Q20" s="6">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>45</v>
       </c>
@@ -2009,58 +2058,58 @@
         <v>67.400000000000006</v>
       </c>
       <c r="E21" s="4">
+        <f t="shared" si="33"/>
+        <v>11.324999999999999</v>
+      </c>
+      <c r="F21" s="5">
+        <f t="shared" si="34"/>
+        <v>25.901535306811454</v>
+      </c>
+      <c r="G21" s="12">
         <f t="shared" si="30"/>
-        <v>11.324999999999999</v>
-      </c>
-      <c r="F21" s="5">
+        <v>22.65</v>
+      </c>
+      <c r="H21" s="5">
+        <f t="shared" si="35"/>
+        <v>44.587785306811455</v>
+      </c>
+      <c r="I21" s="4">
+        <f t="shared" si="36"/>
+        <v>7.55</v>
+      </c>
+      <c r="J21" s="2">
+        <f t="shared" si="37"/>
+        <v>17.267690204540969</v>
+      </c>
+      <c r="K21" s="13">
         <f t="shared" si="31"/>
-        <v>25.901535306811454</v>
-      </c>
-      <c r="G21" s="12">
-        <f>Q21*0.75*C21</f>
-        <v>22.65</v>
-      </c>
-      <c r="H21" s="5">
+        <v>15.1</v>
+      </c>
+      <c r="L21" s="2">
+        <f t="shared" si="38"/>
+        <v>29.725190204540969</v>
+      </c>
+      <c r="M21" s="4">
+        <f t="shared" si="39"/>
+        <v>3.7749999999999999</v>
+      </c>
+      <c r="N21" s="2">
+        <f t="shared" si="40"/>
+        <v>8.6338451022704845</v>
+      </c>
+      <c r="O21" s="13">
         <f t="shared" si="32"/>
-        <v>44.587785306811455</v>
-      </c>
-      <c r="I21" s="4">
-        <f t="shared" si="33"/>
         <v>7.55</v>
       </c>
-      <c r="J21" s="2">
-        <f t="shared" si="34"/>
-        <v>17.267690204540969</v>
-      </c>
-      <c r="K21" s="13">
-        <f>Q21*0.5*C21</f>
-        <v>15.1</v>
-      </c>
-      <c r="L21" s="2">
-        <f t="shared" si="35"/>
-        <v>29.725190204540969</v>
-      </c>
-      <c r="M21" s="4">
-        <f t="shared" si="36"/>
-        <v>3.7749999999999999</v>
-      </c>
-      <c r="N21" s="2">
-        <f t="shared" si="37"/>
-        <v>8.6338451022704845</v>
-      </c>
-      <c r="O21" s="13">
-        <f>Q21*0.25*C21</f>
-        <v>7.55</v>
-      </c>
       <c r="P21" s="2">
-        <f t="shared" si="38"/>
+        <f t="shared" si="41"/>
         <v>14.862595102270484</v>
       </c>
       <c r="Q21" s="6">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>46</v>
       </c>
@@ -2074,51 +2123,51 @@
         <v>25.9</v>
       </c>
       <c r="E22" s="4">
+        <f t="shared" si="33"/>
+        <v>9.375</v>
+      </c>
+      <c r="F22" s="5">
+        <f t="shared" si="34"/>
+        <v>10.784494077146132</v>
+      </c>
+      <c r="G22" s="12">
         <f t="shared" si="30"/>
-        <v>9.375</v>
-      </c>
-      <c r="F22" s="5">
+        <v>18.75</v>
+      </c>
+      <c r="H22" s="5">
+        <f t="shared" si="35"/>
+        <v>26.253244077146132</v>
+      </c>
+      <c r="I22" s="4">
+        <f t="shared" si="36"/>
+        <v>6.25</v>
+      </c>
+      <c r="J22" s="2">
+        <f t="shared" si="37"/>
+        <v>7.1896627180974209</v>
+      </c>
+      <c r="K22" s="13">
         <f t="shared" si="31"/>
-        <v>10.784494077146132</v>
-      </c>
-      <c r="G22" s="12">
-        <f>Q22*0.75*C22</f>
-        <v>18.75</v>
-      </c>
-      <c r="H22" s="5">
+        <v>12.5</v>
+      </c>
+      <c r="L22" s="2">
+        <f t="shared" si="38"/>
+        <v>17.50216271809742</v>
+      </c>
+      <c r="M22" s="4">
+        <f t="shared" si="39"/>
+        <v>3.125</v>
+      </c>
+      <c r="N22" s="2">
+        <f t="shared" si="40"/>
+        <v>3.5948313590487104</v>
+      </c>
+      <c r="O22" s="13">
         <f t="shared" si="32"/>
-        <v>26.253244077146132</v>
-      </c>
-      <c r="I22" s="4">
-        <f t="shared" si="33"/>
         <v>6.25</v>
       </c>
-      <c r="J22" s="2">
-        <f t="shared" si="34"/>
-        <v>7.1896627180974209</v>
-      </c>
-      <c r="K22" s="13">
-        <f>Q22*0.5*C22</f>
-        <v>12.5</v>
-      </c>
-      <c r="L22" s="2">
-        <f t="shared" si="35"/>
-        <v>17.50216271809742</v>
-      </c>
-      <c r="M22" s="4">
-        <f t="shared" si="36"/>
-        <v>3.125</v>
-      </c>
-      <c r="N22" s="2">
-        <f t="shared" si="37"/>
-        <v>3.5948313590487104</v>
-      </c>
-      <c r="O22" s="13">
-        <f>Q22*0.25*C22</f>
-        <v>6.25</v>
-      </c>
       <c r="P22" s="2">
-        <f t="shared" si="38"/>
+        <f t="shared" si="41"/>
         <v>8.75108135904871</v>
       </c>
       <c r="Q22" s="6">

</xml_diff>